<commit_message>
work started on quetta and issue of perfect seperation resolved
</commit_message>
<xml_diff>
--- a/revised/Quetta/Quetta.xlsx
+++ b/revised/Quetta/Quetta.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A80ED2-25F2-4513-BC3D-DE4B85189040}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740BD281-57DB-488F-85D0-29E73BA5B2E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>Year</t>
   </si>
@@ -159,7 +159,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -262,6 +262,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -273,7 +284,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -363,6 +374,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1013,15 +1027,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28029C6-2094-4F19-B9E2-17CE7D370274}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="30">
+    <row r="1" spans="1:4" ht="45">
       <c r="A1" s="21" t="s">
         <v>28</v>
       </c>
@@ -1031,8 +1045,11 @@
       <c r="C1" s="21" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="31">
+      <c r="D1" s="31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="31">
       <c r="A2" s="22" t="s">
         <v>25</v>
       </c>
@@ -1042,8 +1059,11 @@
       <c r="C2" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="46.5">
+      <c r="D2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="46.5">
       <c r="A3" s="22" t="s">
         <v>26</v>
       </c>
@@ -1053,8 +1073,11 @@
       <c r="C3" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="31">
+      <c r="D3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="31">
       <c r="A4" s="22" t="s">
         <v>27</v>
       </c>
@@ -1064,8 +1087,11 @@
       <c r="C4" s="22">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="31">
+      <c r="D4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="31">
       <c r="A5" s="4" t="s">
         <v>24</v>
       </c>
@@ -1073,6 +1099,9 @@
         <v>0</v>
       </c>
       <c r="C5" s="5">
+        <v>14</v>
+      </c>
+      <c r="D5">
         <v>14</v>
       </c>
     </row>

</xml_diff>